<commit_message>
fix(Mise à jour): La colonne "PlanifFt" à étais renommée en "Date cible initiale"
L'attribut [Name] de la propriété PlanifFt dans la classe
ExportInterventionCsv a été renommé de « Planif FT » en « Date cible
initiale ». Ce changement de nom reflète mieux l’intention et
l’utilisation réelles de la propriété.
</commit_message>
<xml_diff>
--- a/LibsPlaningAChaud/Excel/PLANNING VQSE A CHAUD DOSO Z2.xlsx
+++ b/LibsPlaningAChaud/Excel/PLANNING VQSE A CHAUD DOSO Z2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZP6177\Documents\Programmation\C#\GYCsvHelper\LibsPlaningAChaud\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3338C2EC-3297-45A8-85AC-7111A3D279BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A9D479-82AA-4F0B-AED7-C05C06E78212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{13F1EFF0-1EDD-4254-993C-443C98B11AA4}"/>
   </bookViews>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>ND</t>
-  </si>
-  <si>
-    <t>Planif FT</t>
   </si>
   <si>
     <t>UI</t>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>SANANIKONE Ouprasong 06 72 86 90 11</t>
+  </si>
+  <si>
+    <t>Date cible initiale</t>
   </si>
 </sst>
 </file>
@@ -906,31 +906,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
   <dimension ref="A1:K188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,31 +4870,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5844,7 +5844,7 @@
   <dimension ref="A1:K1008"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,31 +5862,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -10936,7 +10936,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10957,31 +10957,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -11100,7 +11100,7 @@
   <dimension ref="A1:K513"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K513"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11116,31 +11116,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -13213,36 +13213,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -13251,13 +13251,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -13266,13 +13266,13 @@
         <v>33</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13281,30 +13281,30 @@
         <v>47</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -13313,13 +13313,13 @@
         <v>24</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -13328,13 +13328,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13343,30 +13343,30 @@
         <v>47</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="24">
         <v>19</v>
       </c>
       <c r="C10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>20</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -13375,13 +13375,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -13390,13 +13390,13 @@
         <v>87</v>
       </c>
       <c r="C12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>20</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -13405,13 +13405,13 @@
         <v>24</v>
       </c>
       <c r="C13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -13420,13 +13420,13 @@
         <v>33</v>
       </c>
       <c r="C14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13435,30 +13435,30 @@
         <v>47</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>19</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -13467,13 +13467,13 @@
         <v>24</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -13482,13 +13482,13 @@
         <v>33</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13497,30 +13497,30 @@
         <v>47</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="24">
         <v>19</v>
       </c>
       <c r="C20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="E20" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -13529,13 +13529,13 @@
         <v>23</v>
       </c>
       <c r="C21" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -13544,13 +13544,13 @@
         <v>24</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -13559,13 +13559,13 @@
         <v>33</v>
       </c>
       <c r="C23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -13574,13 +13574,13 @@
         <v>47</v>
       </c>
       <c r="C24" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13589,13 +13589,13 @@
         <v>87</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="E25" s="35" t="s">
         <v>46</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>